<commit_message>
ultim debug of calculus tree
</commit_message>
<xml_diff>
--- a/web/simulator/result/simulation_1.xlsx
+++ b/web/simulator/result/simulation_1.xlsx
@@ -1307,9 +1307,7 @@
           <t>Project Duration</t>
         </is>
       </c>
-      <c r="F16" s="43" t="n">
-        <v>10</v>
-      </c>
+      <c r="F16" s="43" t="inlineStr"/>
       <c r="G16" s="38" t="inlineStr">
         <is>
           <t>years</t>
@@ -1754,9 +1752,7 @@
           <t>%</t>
         </is>
       </c>
-      <c r="J49" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
+      <c r="J49" s="43" t="inlineStr"/>
       <c r="K49" t="inlineStr">
         <is>
           <t>%</t>
@@ -1788,442 +1784,376 @@
       </c>
     </row>
     <row r="50" ht="20" customHeight="1">
-      <c r="F50" s="50" t="n">
+      <c r="F50" t="n">
         <v>0.04</v>
       </c>
-      <c r="H50" s="50" t="n">
+      <c r="H50" t="n">
         <v>0.01</v>
       </c>
-      <c r="J50" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
-      <c r="L50" s="50" t="n">
+      <c r="L50" t="n">
         <v>10</v>
       </c>
-      <c r="N50" s="67" t="n">
+      <c r="N50" t="n">
         <v>25</v>
       </c>
-      <c r="P50" s="67" t="n">
+      <c r="P50" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="51" ht="20" customHeight="1">
-      <c r="F51" s="50" t="n">
+      <c r="F51" t="n">
         <v>0.04</v>
       </c>
-      <c r="H51" s="50" t="n">
+      <c r="H51" t="n">
         <v>0.26</v>
       </c>
-      <c r="J51" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
-      <c r="L51" s="50" t="n">
+      <c r="L51" t="n">
         <v>10.333</v>
       </c>
-      <c r="N51" s="67" t="n">
+      <c r="N51" t="n">
         <v>26.556</v>
       </c>
-      <c r="P51" s="67" t="n">
+      <c r="P51" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="52" ht="20" customHeight="1">
-      <c r="F52" s="50" t="n">
+      <c r="F52" t="n">
         <v>0.04</v>
       </c>
-      <c r="H52" s="50" t="n">
+      <c r="H52" t="n">
         <v>0.509</v>
       </c>
-      <c r="J52" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
-      <c r="L52" s="50" t="n">
+      <c r="L52" t="n">
         <v>10.667</v>
       </c>
-      <c r="N52" s="67" t="n">
+      <c r="N52" t="n">
         <v>28.111</v>
       </c>
-      <c r="P52" s="67" t="n">
+      <c r="P52" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="53" ht="20" customHeight="1">
-      <c r="F53" s="50" t="n">
+      <c r="F53" t="n">
         <v>0.04</v>
       </c>
-      <c r="H53" s="50" t="n">
+      <c r="H53" t="n">
         <v>0.758</v>
       </c>
-      <c r="J53" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
-      <c r="L53" s="50" t="n">
+      <c r="L53" t="n">
         <v>11</v>
       </c>
-      <c r="N53" s="67" t="n">
+      <c r="N53" t="n">
         <v>29.667</v>
       </c>
-      <c r="P53" s="67" t="n">
+      <c r="P53" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="54" ht="20" customHeight="1">
-      <c r="F54" s="50" t="n">
+      <c r="F54" t="n">
         <v>0.04</v>
       </c>
-      <c r="H54" s="50" t="n">
+      <c r="H54" t="n">
         <v>1.008</v>
       </c>
-      <c r="J54" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
-      <c r="L54" s="50" t="n">
+      <c r="L54" t="n">
         <v>11.333</v>
       </c>
-      <c r="N54" s="67" t="n">
+      <c r="N54" t="n">
         <v>31.222</v>
       </c>
-      <c r="P54" s="67" t="n">
+      <c r="P54" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="55" ht="20" customHeight="1">
-      <c r="F55" s="50" t="n">
+      <c r="F55" t="n">
         <v>0.04</v>
       </c>
-      <c r="H55" s="50" t="n">
+      <c r="H55" t="n">
         <v>1.258</v>
       </c>
-      <c r="J55" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
-      <c r="L55" s="50" t="n">
+      <c r="L55" t="n">
         <v>11.667</v>
       </c>
-      <c r="N55" s="67" t="n">
+      <c r="N55" t="n">
         <v>32.778</v>
       </c>
-      <c r="P55" s="67" t="n">
+      <c r="P55" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="56" ht="20" customHeight="1">
-      <c r="F56" s="50" t="n">
+      <c r="F56" t="n">
         <v>0.04</v>
       </c>
-      <c r="H56" s="50" t="n">
+      <c r="H56" t="n">
         <v>1.507</v>
       </c>
-      <c r="J56" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
-      <c r="L56" s="50" t="n">
+      <c r="L56" t="n">
         <v>12</v>
       </c>
-      <c r="N56" s="67" t="n">
+      <c r="N56" t="n">
         <v>34.333</v>
       </c>
-      <c r="P56" s="67" t="n">
+      <c r="P56" t="n">
         <v>22</v>
       </c>
     </row>
     <row r="57" ht="20" customHeight="1">
-      <c r="F57" s="50" t="n">
+      <c r="F57" t="n">
         <v>0.04</v>
       </c>
-      <c r="H57" s="50" t="n">
+      <c r="H57" t="n">
         <v>1.756</v>
       </c>
-      <c r="J57" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
-      <c r="L57" s="50" t="n">
+      <c r="L57" t="n">
         <v>12.333</v>
       </c>
-      <c r="N57" s="67" t="n">
+      <c r="N57" t="n">
         <v>35.889</v>
       </c>
-      <c r="P57" s="67" t="n">
+      <c r="P57" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="58" ht="20" customHeight="1">
-      <c r="F58" s="50" t="n">
+      <c r="F58" t="n">
         <v>0.04</v>
       </c>
-      <c r="H58" s="50" t="n">
+      <c r="H58" t="n">
         <v>2.006</v>
       </c>
-      <c r="J58" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
-      <c r="L58" s="50" t="n">
+      <c r="L58" t="n">
         <v>12.667</v>
       </c>
-      <c r="N58" s="67" t="n">
+      <c r="N58" t="n">
         <v>37.444</v>
       </c>
-      <c r="P58" s="67" t="n">
+      <c r="P58" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="59" ht="20" customHeight="1">
-      <c r="F59" s="50" t="n">
+      <c r="F59" t="n">
         <v>0.04</v>
       </c>
-      <c r="H59" s="50" t="n">
+      <c r="H59" t="n">
         <v>2.255</v>
       </c>
-      <c r="J59" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
-      <c r="L59" s="50" t="n">
+      <c r="L59" t="n">
         <v>13</v>
       </c>
-      <c r="N59" s="67" t="n">
+      <c r="N59" t="n">
         <v>39</v>
       </c>
-      <c r="P59" s="67" t="n">
+      <c r="P59" t="n">
         <v>28</v>
       </c>
     </row>
     <row r="60" ht="20" customHeight="1">
-      <c r="F60" s="50" t="n">
+      <c r="F60" t="n">
         <v>0.04</v>
       </c>
-      <c r="H60" s="50" t="n">
+      <c r="H60" t="n">
         <v>2.505</v>
       </c>
-      <c r="J60" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
-      <c r="L60" s="50" t="n">
+      <c r="L60" t="n">
         <v>13.333</v>
       </c>
-      <c r="N60" s="67" t="n">
+      <c r="N60" t="n">
         <v>40.556</v>
       </c>
-      <c r="P60" s="67" t="n">
+      <c r="P60" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="61" ht="20" customHeight="1">
-      <c r="F61" s="50" t="n">
+      <c r="F61" t="n">
         <v>0.04</v>
       </c>
-      <c r="H61" s="50" t="n">
+      <c r="H61" t="n">
         <v>2.754</v>
       </c>
-      <c r="J61" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
-      <c r="L61" s="50" t="n">
+      <c r="L61" t="n">
         <v>13.667</v>
       </c>
-      <c r="N61" s="67" t="n">
+      <c r="N61" t="n">
         <v>42.111</v>
       </c>
-      <c r="P61" s="67" t="n">
+      <c r="P61" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="62" ht="20" customHeight="1">
-      <c r="F62" s="50" t="n">
+      <c r="F62" t="n">
         <v>0.04</v>
       </c>
-      <c r="H62" s="50" t="n">
+      <c r="H62" t="n">
         <v>3.004</v>
       </c>
-      <c r="J62" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
-      <c r="L62" s="50" t="n">
+      <c r="L62" t="n">
         <v>14</v>
       </c>
-      <c r="N62" s="67" t="n">
+      <c r="N62" t="n">
         <v>43.667</v>
       </c>
-      <c r="P62" s="67" t="n">
+      <c r="P62" t="n">
         <v>34</v>
       </c>
     </row>
     <row r="63" ht="20" customHeight="1">
-      <c r="F63" s="50" t="n">
+      <c r="F63" t="n">
         <v>0.04</v>
       </c>
-      <c r="H63" s="50" t="n">
+      <c r="H63" t="n">
         <v>3.253</v>
       </c>
-      <c r="J63" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
-      <c r="L63" s="50" t="n">
+      <c r="L63" t="n">
         <v>14.333</v>
       </c>
-      <c r="N63" s="67" t="n">
+      <c r="N63" t="n">
         <v>45.222</v>
       </c>
-      <c r="P63" s="67" t="n">
+      <c r="P63" t="n">
         <v>36</v>
       </c>
     </row>
     <row r="64" ht="20" customHeight="1">
-      <c r="F64" s="50" t="n">
+      <c r="F64" t="n">
         <v>0.04</v>
       </c>
-      <c r="H64" s="50" t="n">
+      <c r="H64" t="n">
         <v>3.503</v>
       </c>
-      <c r="J64" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
-      <c r="L64" s="50" t="n">
+      <c r="L64" t="n">
         <v>14.667</v>
       </c>
-      <c r="N64" s="67" t="n">
+      <c r="N64" t="n">
         <v>46.778</v>
       </c>
-      <c r="P64" s="67" t="n">
+      <c r="P64" t="n">
         <v>38</v>
       </c>
     </row>
     <row r="65" ht="20" customHeight="1">
-      <c r="F65" s="50" t="n">
+      <c r="F65" t="n">
         <v>0.04</v>
       </c>
-      <c r="H65" s="50" t="n">
+      <c r="H65" t="n">
         <v>3.752</v>
       </c>
-      <c r="J65" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
-      <c r="L65" s="50" t="n">
+      <c r="L65" t="n">
         <v>15</v>
       </c>
-      <c r="N65" s="67" t="n">
+      <c r="N65" t="n">
         <v>48.333</v>
       </c>
-      <c r="P65" s="67" t="n">
+      <c r="P65" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="66" ht="20" customHeight="1">
-      <c r="F66" s="50" t="n">
+      <c r="F66" t="n">
         <v>0.04</v>
       </c>
-      <c r="H66" s="50" t="n">
+      <c r="H66" t="n">
         <v>4.002</v>
       </c>
-      <c r="J66" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
-      <c r="L66" s="50" t="n">
+      <c r="L66" t="n">
         <v>15.333</v>
       </c>
-      <c r="N66" s="67" t="n">
+      <c r="N66" t="n">
         <v>49.889</v>
       </c>
-      <c r="P66" s="67" t="n">
+      <c r="P66" t="n">
         <v>42</v>
       </c>
     </row>
     <row r="67" ht="20" customHeight="1">
-      <c r="F67" s="50" t="n">
+      <c r="F67" t="n">
         <v>0.04</v>
       </c>
-      <c r="H67" s="50" t="n">
+      <c r="H67" t="n">
         <v>4.252</v>
       </c>
-      <c r="J67" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
-      <c r="L67" s="50" t="n">
+      <c r="L67" t="n">
         <v>15.667</v>
       </c>
-      <c r="N67" s="67" t="n">
+      <c r="N67" t="n">
         <v>51.444</v>
       </c>
-      <c r="P67" s="67" t="n">
+      <c r="P67" t="n">
         <v>44</v>
       </c>
     </row>
     <row r="68" ht="31" customHeight="1">
-      <c r="F68" s="50" t="n">
+      <c r="F68" t="n">
         <v>0.04</v>
       </c>
-      <c r="H68" s="50" t="n">
+      <c r="H68" t="n">
         <v>4.501</v>
       </c>
-      <c r="J68" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
-      <c r="L68" s="50" t="n">
+      <c r="L68" t="n">
         <v>16</v>
       </c>
-      <c r="N68" s="67" t="n">
+      <c r="N68" t="n">
         <v>53</v>
       </c>
-      <c r="P68" s="67" t="n">
+      <c r="P68" t="n">
         <v>46</v>
       </c>
     </row>
     <row r="69" ht="47" customHeight="1">
-      <c r="F69" s="50" t="n">
+      <c r="F69" t="n">
         <v>0.04</v>
       </c>
-      <c r="H69" s="50" t="n">
+      <c r="H69" t="n">
         <v>4.75</v>
       </c>
-      <c r="J69" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
-      <c r="L69" s="50" t="n">
+      <c r="L69" t="n">
         <v>16.333</v>
       </c>
-      <c r="N69" s="67" t="n">
+      <c r="N69" t="n">
         <v>54.556</v>
       </c>
-      <c r="P69" s="67" t="n">
+      <c r="P69" t="n">
         <v>48</v>
       </c>
     </row>
     <row r="70" ht="20" customHeight="1">
-      <c r="F70" s="50" t="n">
+      <c r="F70" t="n">
         <v>0.04</v>
       </c>
-      <c r="H70" s="50" t="n">
+      <c r="H70" t="n">
         <v>5</v>
       </c>
-      <c r="J70" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
-      <c r="L70" s="50" t="n">
+      <c r="L70" t="n">
         <v>16.667</v>
       </c>
-      <c r="N70" s="67" t="n">
+      <c r="N70" t="n">
         <v>56.111</v>
       </c>
-      <c r="P70" s="67" t="n">
+      <c r="P70" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="71" ht="20" customHeight="1">
-      <c r="F71" s="50" t="n">
+      <c r="F71" t="n">
         <v>0.04</v>
       </c>
-      <c r="H71" s="50" t="n">
+      <c r="H71" t="n">
         <v>5.249</v>
       </c>
-      <c r="J71" s="43" t="n">
-        <v>-0.713469919350799</v>
-      </c>
-      <c r="L71" s="50" t="n">
+      <c r="L71" t="n">
         <v>17</v>
       </c>
-      <c r="N71" s="67" t="n">
+      <c r="N71" t="n">
         <v>57.667</v>
       </c>
-      <c r="P71" s="67" t="n">
+      <c r="P71" t="n">
         <v>52</v>
       </c>
     </row>
@@ -2600,970 +2530,970 @@
       </c>
     </row>
     <row r="79" ht="20" customHeight="1">
-      <c r="F79" s="34" t="n">
+      <c r="F79" t="n">
         <v>2350</v>
       </c>
-      <c r="G79" s="34" t="n">
+      <c r="G79" t="n">
         <v>4220</v>
       </c>
-      <c r="I79" s="34" t="n">
+      <c r="I79" t="n">
         <v>65</v>
       </c>
-      <c r="J79" s="34" t="n">
+      <c r="J79" t="n">
         <v>65</v>
       </c>
-      <c r="L79" s="34" t="n">
+      <c r="L79" t="n">
         <v>10</v>
       </c>
-      <c r="M79" s="34" t="n">
+      <c r="M79" t="n">
         <v>10</v>
       </c>
-      <c r="O79" s="34" t="n">
+      <c r="O79" t="n">
         <v>896</v>
       </c>
-      <c r="P79" s="34" t="n">
+      <c r="P79" t="n">
         <v>896</v>
       </c>
-      <c r="R79" s="76" t="n">
+      <c r="R79" t="n">
         <v>1</v>
       </c>
-      <c r="S79" s="76" t="n">
+      <c r="S79" t="n">
         <v>0.85</v>
       </c>
-      <c r="U79" s="34" t="n">
+      <c r="U79" t="n">
         <v>3.625</v>
       </c>
-      <c r="V79" s="34" t="n">
+      <c r="V79" t="n">
         <v>4</v>
       </c>
-      <c r="X79" s="34" t="n">
+      <c r="X79" t="n">
         <v>0.17</v>
       </c>
-      <c r="Y79" s="34" t="n">
+      <c r="Y79" t="n">
         <v>0.3</v>
       </c>
     </row>
     <row r="80" ht="20" customHeight="1">
-      <c r="F80" s="34" t="n">
+      <c r="F80" t="n">
         <v>2581.657</v>
       </c>
-      <c r="G80" s="34" t="n">
+      <c r="G80" t="n">
         <v>4429.191</v>
       </c>
-      <c r="I80" s="34" t="n">
+      <c r="I80" t="n">
         <v>65</v>
       </c>
-      <c r="J80" s="34" t="n">
+      <c r="J80" t="n">
         <v>65</v>
       </c>
-      <c r="L80" s="34" t="n">
+      <c r="L80" t="n">
         <v>11</v>
       </c>
-      <c r="M80" s="34" t="n">
+      <c r="M80" t="n">
         <v>11</v>
       </c>
-      <c r="O80" s="34" t="n">
+      <c r="O80" t="n">
         <v>896</v>
       </c>
-      <c r="P80" s="34" t="n">
+      <c r="P80" t="n">
         <v>896</v>
       </c>
-      <c r="R80" s="76" t="n">
+      <c r="R80" t="n">
         <v>1</v>
       </c>
-      <c r="S80" s="76" t="n">
+      <c r="S80" t="n">
         <v>0.85</v>
       </c>
-      <c r="U80" s="34" t="n">
+      <c r="U80" t="n">
         <v>3.625</v>
       </c>
-      <c r="V80" s="34" t="n">
+      <c r="V80" t="n">
         <v>4</v>
       </c>
-      <c r="X80" s="34" t="n">
+      <c r="X80" t="n">
         <v>0.289</v>
       </c>
-      <c r="Y80" s="34" t="n">
+      <c r="Y80" t="n">
         <v>0.471</v>
       </c>
     </row>
     <row r="81" ht="20" customHeight="1">
-      <c r="F81" s="34" t="n">
+      <c r="F81" t="n">
         <v>2823.77</v>
       </c>
-      <c r="G81" s="34" t="n">
+      <c r="G81" t="n">
         <v>4638.298</v>
       </c>
-      <c r="I81" s="34" t="n">
+      <c r="I81" t="n">
         <v>65</v>
       </c>
-      <c r="J81" s="34" t="n">
+      <c r="J81" t="n">
         <v>65</v>
       </c>
-      <c r="L81" s="34" t="n">
+      <c r="L81" t="n">
         <v>12</v>
       </c>
-      <c r="M81" s="34" t="n">
+      <c r="M81" t="n">
         <v>12</v>
       </c>
-      <c r="O81" s="34" t="n">
+      <c r="O81" t="n">
         <v>896</v>
       </c>
-      <c r="P81" s="34" t="n">
+      <c r="P81" t="n">
         <v>896</v>
       </c>
-      <c r="R81" s="76" t="n">
+      <c r="R81" t="n">
         <v>1</v>
       </c>
-      <c r="S81" s="76" t="n">
+      <c r="S81" t="n">
         <v>0.85</v>
       </c>
-      <c r="U81" s="34" t="n">
+      <c r="U81" t="n">
         <v>3.625</v>
       </c>
-      <c r="V81" s="34" t="n">
+      <c r="V81" t="n">
         <v>4</v>
       </c>
-      <c r="X81" s="34" t="n">
+      <c r="X81" t="n">
         <v>0.407</v>
       </c>
-      <c r="Y81" s="34" t="n">
+      <c r="Y81" t="n">
         <v>0.643</v>
       </c>
     </row>
     <row r="82" ht="20" customHeight="1">
-      <c r="F82" s="34" t="n">
+      <c r="F82" t="n">
         <v>3076.305</v>
       </c>
-      <c r="G82" s="34" t="n">
+      <c r="G82" t="n">
         <v>4847.326</v>
       </c>
-      <c r="I82" s="34" t="n">
+      <c r="I82" t="n">
         <v>65</v>
       </c>
-      <c r="J82" s="34" t="n">
+      <c r="J82" t="n">
         <v>65</v>
       </c>
-      <c r="L82" s="34" t="n">
+      <c r="L82" t="n">
         <v>13</v>
       </c>
-      <c r="M82" s="34" t="n">
+      <c r="M82" t="n">
         <v>13</v>
       </c>
-      <c r="O82" s="34" t="n">
+      <c r="O82" t="n">
         <v>896</v>
       </c>
-      <c r="P82" s="34" t="n">
+      <c r="P82" t="n">
         <v>896</v>
       </c>
-      <c r="R82" s="76" t="n">
+      <c r="R82" t="n">
         <v>1</v>
       </c>
-      <c r="S82" s="76" t="n">
+      <c r="S82" t="n">
         <v>0.85</v>
       </c>
-      <c r="U82" s="34" t="n">
+      <c r="U82" t="n">
         <v>3.625</v>
       </c>
-      <c r="V82" s="34" t="n">
+      <c r="V82" t="n">
         <v>4</v>
       </c>
-      <c r="X82" s="34" t="n">
+      <c r="X82" t="n">
         <v>0.526</v>
       </c>
-      <c r="Y82" s="34" t="n">
+      <c r="Y82" t="n">
         <v>0.8139999999999999</v>
       </c>
     </row>
     <row r="83" ht="20" customHeight="1">
-      <c r="F83" s="34" t="n">
+      <c r="F83" t="n">
         <v>3339.226</v>
       </c>
-      <c r="G83" s="34" t="n">
+      <c r="G83" t="n">
         <v>5056.278</v>
       </c>
-      <c r="I83" s="34" t="n">
+      <c r="I83" t="n">
         <v>65</v>
       </c>
-      <c r="J83" s="34" t="n">
+      <c r="J83" t="n">
         <v>65</v>
       </c>
-      <c r="L83" s="34" t="n">
+      <c r="L83" t="n">
         <v>14</v>
       </c>
-      <c r="M83" s="34" t="n">
+      <c r="M83" t="n">
         <v>14</v>
       </c>
-      <c r="O83" s="34" t="n">
+      <c r="O83" t="n">
         <v>896</v>
       </c>
-      <c r="P83" s="34" t="n">
+      <c r="P83" t="n">
         <v>896</v>
       </c>
-      <c r="R83" s="76" t="n">
+      <c r="R83" t="n">
         <v>1</v>
       </c>
-      <c r="S83" s="76" t="n">
+      <c r="S83" t="n">
         <v>0.85</v>
       </c>
-      <c r="U83" s="34" t="n">
+      <c r="U83" t="n">
         <v>3.625</v>
       </c>
-      <c r="V83" s="34" t="n">
+      <c r="V83" t="n">
         <v>4</v>
       </c>
-      <c r="X83" s="34" t="n">
+      <c r="X83" t="n">
         <v>0.644</v>
       </c>
-      <c r="Y83" s="34" t="n">
+      <c r="Y83" t="n">
         <v>0.986</v>
       </c>
     </row>
     <row r="84" ht="20" customHeight="1">
-      <c r="F84" s="34" t="n">
+      <c r="F84" t="n">
         <v>3612.503</v>
       </c>
-      <c r="G84" s="34" t="n">
+      <c r="G84" t="n">
         <v>5265.157</v>
       </c>
-      <c r="I84" s="34" t="n">
+      <c r="I84" t="n">
         <v>65</v>
       </c>
-      <c r="J84" s="34" t="n">
+      <c r="J84" t="n">
         <v>65</v>
       </c>
-      <c r="L84" s="34" t="n">
+      <c r="L84" t="n">
         <v>15</v>
       </c>
-      <c r="M84" s="34" t="n">
+      <c r="M84" t="n">
         <v>15</v>
       </c>
-      <c r="O84" s="34" t="n">
+      <c r="O84" t="n">
         <v>896</v>
       </c>
-      <c r="P84" s="34" t="n">
+      <c r="P84" t="n">
         <v>896</v>
       </c>
-      <c r="R84" s="76" t="n">
+      <c r="R84" t="n">
         <v>1</v>
       </c>
-      <c r="S84" s="76" t="n">
+      <c r="S84" t="n">
         <v>0.85</v>
       </c>
-      <c r="U84" s="34" t="n">
+      <c r="U84" t="n">
         <v>3.625</v>
       </c>
-      <c r="V84" s="34" t="n">
+      <c r="V84" t="n">
         <v>4</v>
       </c>
-      <c r="X84" s="34" t="n">
+      <c r="X84" t="n">
         <v>0.763</v>
       </c>
-      <c r="Y84" s="34" t="n">
+      <c r="Y84" t="n">
         <v>1.157</v>
       </c>
     </row>
     <row r="85" ht="20" customHeight="1">
-      <c r="F85" s="34" t="n">
+      <c r="F85" t="n">
         <v>3896.104</v>
       </c>
-      <c r="G85" s="34" t="n">
+      <c r="G85" t="n">
         <v>5473.966</v>
       </c>
-      <c r="I85" s="34" t="n">
+      <c r="I85" t="n">
         <v>65</v>
       </c>
-      <c r="J85" s="34" t="n">
+      <c r="J85" t="n">
         <v>65</v>
       </c>
-      <c r="L85" s="34" t="n">
+      <c r="L85" t="n">
         <v>16</v>
       </c>
-      <c r="M85" s="34" t="n">
+      <c r="M85" t="n">
         <v>16</v>
       </c>
-      <c r="O85" s="34" t="n">
+      <c r="O85" t="n">
         <v>896</v>
       </c>
-      <c r="P85" s="34" t="n">
+      <c r="P85" t="n">
         <v>896</v>
       </c>
-      <c r="R85" s="76" t="n">
+      <c r="R85" t="n">
         <v>1</v>
       </c>
-      <c r="S85" s="76" t="n">
+      <c r="S85" t="n">
         <v>0.85</v>
       </c>
-      <c r="U85" s="34" t="n">
+      <c r="U85" t="n">
         <v>3.625</v>
       </c>
-      <c r="V85" s="34" t="n">
+      <c r="V85" t="n">
         <v>4</v>
       </c>
-      <c r="X85" s="34" t="n">
+      <c r="X85" t="n">
         <v>0.881</v>
       </c>
-      <c r="Y85" s="34" t="n">
+      <c r="Y85" t="n">
         <v>1.329</v>
       </c>
     </row>
     <row r="86" ht="20" customHeight="1">
-      <c r="F86" s="34" t="n">
+      <c r="F86" t="n">
         <v>4190</v>
       </c>
-      <c r="G86" s="34" t="n">
+      <c r="G86" t="n">
         <v>5682.708</v>
       </c>
-      <c r="I86" s="34" t="n">
+      <c r="I86" t="n">
         <v>65</v>
       </c>
-      <c r="J86" s="34" t="n">
+      <c r="J86" t="n">
         <v>65</v>
       </c>
-      <c r="L86" s="34" t="n">
+      <c r="L86" t="n">
         <v>17</v>
       </c>
-      <c r="M86" s="34" t="n">
+      <c r="M86" t="n">
         <v>17</v>
       </c>
-      <c r="O86" s="34" t="n">
+      <c r="O86" t="n">
         <v>896</v>
       </c>
-      <c r="P86" s="34" t="n">
+      <c r="P86" t="n">
         <v>896</v>
       </c>
-      <c r="R86" s="76" t="n">
+      <c r="R86" t="n">
         <v>1</v>
       </c>
-      <c r="S86" s="76" t="n">
+      <c r="S86" t="n">
         <v>0.85</v>
       </c>
-      <c r="U86" s="34" t="n">
+      <c r="U86" t="n">
         <v>3.625</v>
       </c>
-      <c r="V86" s="34" t="n">
+      <c r="V86" t="n">
         <v>4</v>
       </c>
-      <c r="X86" s="34" t="n">
+      <c r="X86" t="n">
         <v>1</v>
       </c>
-      <c r="Y86" s="34" t="n">
+      <c r="Y86" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="87" ht="20" customHeight="1">
-      <c r="F87" s="34" t="n">
+      <c r="F87" t="n">
         <v>4494.162</v>
       </c>
-      <c r="G87" s="34" t="n">
+      <c r="G87" t="n">
         <v>5891.385</v>
       </c>
-      <c r="I87" s="34" t="n">
+      <c r="I87" t="n">
         <v>65</v>
       </c>
-      <c r="J87" s="34" t="n">
+      <c r="J87" t="n">
         <v>65</v>
       </c>
-      <c r="L87" s="34" t="n">
+      <c r="L87" t="n">
         <v>18</v>
       </c>
-      <c r="M87" s="34" t="n">
+      <c r="M87" t="n">
         <v>18</v>
       </c>
-      <c r="O87" s="34" t="n">
+      <c r="O87" t="n">
         <v>896</v>
       </c>
-      <c r="P87" s="34" t="n">
+      <c r="P87" t="n">
         <v>896</v>
       </c>
-      <c r="R87" s="76" t="n">
+      <c r="R87" t="n">
         <v>1</v>
       </c>
-      <c r="S87" s="76" t="n">
+      <c r="S87" t="n">
         <v>0.85</v>
       </c>
-      <c r="U87" s="34" t="n">
+      <c r="U87" t="n">
         <v>3.625</v>
       </c>
-      <c r="V87" s="34" t="n">
+      <c r="V87" t="n">
         <v>4</v>
       </c>
-      <c r="X87" s="34" t="n">
+      <c r="X87" t="n">
         <v>1.119</v>
       </c>
-      <c r="Y87" s="34" t="n">
+      <c r="Y87" t="n">
         <v>1.671</v>
       </c>
     </row>
     <row r="88" ht="20" customHeight="1">
-      <c r="F88" s="34" t="n">
+      <c r="F88" t="n">
         <v>4808.563</v>
       </c>
-      <c r="G88" s="34" t="n">
+      <c r="G88" t="n">
         <v>6100</v>
       </c>
-      <c r="I88" s="34" t="n">
+      <c r="I88" t="n">
         <v>65</v>
       </c>
-      <c r="J88" s="34" t="n">
+      <c r="J88" t="n">
         <v>65</v>
       </c>
-      <c r="L88" s="34" t="n">
+      <c r="L88" t="n">
         <v>19</v>
       </c>
-      <c r="M88" s="34" t="n">
+      <c r="M88" t="n">
         <v>19</v>
       </c>
-      <c r="O88" s="34" t="n">
+      <c r="O88" t="n">
         <v>896</v>
       </c>
-      <c r="P88" s="34" t="n">
+      <c r="P88" t="n">
         <v>896</v>
       </c>
-      <c r="R88" s="76" t="n">
+      <c r="R88" t="n">
         <v>1</v>
       </c>
-      <c r="S88" s="76" t="n">
+      <c r="S88" t="n">
         <v>0.85</v>
       </c>
-      <c r="U88" s="34" t="n">
+      <c r="U88" t="n">
         <v>3.625</v>
       </c>
-      <c r="V88" s="34" t="n">
+      <c r="V88" t="n">
         <v>4</v>
       </c>
-      <c r="X88" s="34" t="n">
+      <c r="X88" t="n">
         <v>1.237</v>
       </c>
-      <c r="Y88" s="34" t="n">
+      <c r="Y88" t="n">
         <v>1.843</v>
       </c>
     </row>
     <row r="89" ht="20" customHeight="1">
-      <c r="F89" s="34" t="n">
+      <c r="F89" t="n">
         <v>5133.177</v>
       </c>
-      <c r="G89" s="34" t="n">
+      <c r="G89" t="n">
         <v>6308.555</v>
       </c>
-      <c r="I89" s="34" t="n">
+      <c r="I89" t="n">
         <v>65</v>
       </c>
-      <c r="J89" s="34" t="n">
+      <c r="J89" t="n">
         <v>65</v>
       </c>
-      <c r="L89" s="34" t="n">
+      <c r="L89" t="n">
         <v>20</v>
       </c>
-      <c r="M89" s="34" t="n">
+      <c r="M89" t="n">
         <v>20</v>
       </c>
-      <c r="O89" s="34" t="n">
+      <c r="O89" t="n">
         <v>896</v>
       </c>
-      <c r="P89" s="34" t="n">
+      <c r="P89" t="n">
         <v>896</v>
       </c>
-      <c r="R89" s="76" t="n">
+      <c r="R89" t="n">
         <v>1</v>
       </c>
-      <c r="S89" s="76" t="n">
+      <c r="S89" t="n">
         <v>0.85</v>
       </c>
-      <c r="U89" s="34" t="n">
+      <c r="U89" t="n">
         <v>3.625</v>
       </c>
-      <c r="V89" s="34" t="n">
+      <c r="V89" t="n">
         <v>4</v>
       </c>
-      <c r="X89" s="34" t="n">
+      <c r="X89" t="n">
         <v>1.356</v>
       </c>
-      <c r="Y89" s="34" t="n">
+      <c r="Y89" t="n">
         <v>2.014</v>
       </c>
     </row>
     <row r="90" ht="20" customHeight="1">
-      <c r="F90" s="34" t="n">
+      <c r="F90" t="n">
         <v>5467.979</v>
       </c>
-      <c r="G90" s="34" t="n">
+      <c r="G90" t="n">
         <v>6517.051</v>
       </c>
-      <c r="I90" s="34" t="n">
+      <c r="I90" t="n">
         <v>65</v>
       </c>
-      <c r="J90" s="34" t="n">
+      <c r="J90" t="n">
         <v>65</v>
       </c>
-      <c r="L90" s="34" t="n">
+      <c r="L90" t="n">
         <v>21</v>
       </c>
-      <c r="M90" s="34" t="n">
+      <c r="M90" t="n">
         <v>21</v>
       </c>
-      <c r="O90" s="34" t="n">
+      <c r="O90" t="n">
         <v>896</v>
       </c>
-      <c r="P90" s="34" t="n">
+      <c r="P90" t="n">
         <v>896</v>
       </c>
-      <c r="R90" s="76" t="n">
+      <c r="R90" t="n">
         <v>1</v>
       </c>
-      <c r="S90" s="76" t="n">
+      <c r="S90" t="n">
         <v>0.85</v>
       </c>
-      <c r="U90" s="34" t="n">
+      <c r="U90" t="n">
         <v>3.625</v>
       </c>
-      <c r="V90" s="34" t="n">
+      <c r="V90" t="n">
         <v>4</v>
       </c>
-      <c r="X90" s="34" t="n">
+      <c r="X90" t="n">
         <v>1.474</v>
       </c>
-      <c r="Y90" s="34" t="n">
+      <c r="Y90" t="n">
         <v>2.186</v>
       </c>
     </row>
     <row r="91" ht="20" customHeight="1">
-      <c r="F91" s="34" t="n">
+      <c r="F91" t="n">
         <v>5812.943</v>
       </c>
-      <c r="G91" s="34" t="n">
+      <c r="G91" t="n">
         <v>6725.491</v>
       </c>
-      <c r="I91" s="34" t="n">
+      <c r="I91" t="n">
         <v>65</v>
       </c>
-      <c r="J91" s="34" t="n">
+      <c r="J91" t="n">
         <v>65</v>
       </c>
-      <c r="L91" s="34" t="n">
+      <c r="L91" t="n">
         <v>22</v>
       </c>
-      <c r="M91" s="34" t="n">
+      <c r="M91" t="n">
         <v>22</v>
       </c>
-      <c r="O91" s="34" t="n">
+      <c r="O91" t="n">
         <v>896</v>
       </c>
-      <c r="P91" s="34" t="n">
+      <c r="P91" t="n">
         <v>896</v>
       </c>
-      <c r="R91" s="76" t="n">
+      <c r="R91" t="n">
         <v>1</v>
       </c>
-      <c r="S91" s="76" t="n">
+      <c r="S91" t="n">
         <v>0.85</v>
       </c>
-      <c r="U91" s="34" t="n">
+      <c r="U91" t="n">
         <v>3.625</v>
       </c>
-      <c r="V91" s="34" t="n">
+      <c r="V91" t="n">
         <v>4</v>
       </c>
-      <c r="X91" s="34" t="n">
+      <c r="X91" t="n">
         <v>1.593</v>
       </c>
-      <c r="Y91" s="34" t="n">
+      <c r="Y91" t="n">
         <v>2.357</v>
       </c>
     </row>
     <row r="92" ht="20" customHeight="1">
-      <c r="F92" s="34" t="n">
+      <c r="F92" t="n">
         <v>6168.048</v>
       </c>
-      <c r="G92" s="34" t="n">
+      <c r="G92" t="n">
         <v>6933.876</v>
       </c>
-      <c r="I92" s="34" t="n">
+      <c r="I92" t="n">
         <v>65</v>
       </c>
-      <c r="J92" s="34" t="n">
+      <c r="J92" t="n">
         <v>65</v>
       </c>
-      <c r="L92" s="34" t="n">
+      <c r="L92" t="n">
         <v>23</v>
       </c>
-      <c r="M92" s="34" t="n">
+      <c r="M92" t="n">
         <v>23</v>
       </c>
-      <c r="O92" s="34" t="n">
+      <c r="O92" t="n">
         <v>896</v>
       </c>
-      <c r="P92" s="34" t="n">
+      <c r="P92" t="n">
         <v>896</v>
       </c>
-      <c r="R92" s="76" t="n">
+      <c r="R92" t="n">
         <v>1</v>
       </c>
-      <c r="S92" s="76" t="n">
+      <c r="S92" t="n">
         <v>0.85</v>
       </c>
-      <c r="U92" s="34" t="n">
+      <c r="U92" t="n">
         <v>3.625</v>
       </c>
-      <c r="V92" s="34" t="n">
+      <c r="V92" t="n">
         <v>4</v>
       </c>
-      <c r="X92" s="34" t="n">
+      <c r="X92" t="n">
         <v>1.711</v>
       </c>
-      <c r="Y92" s="34" t="n">
+      <c r="Y92" t="n">
         <v>2.529</v>
       </c>
     </row>
     <row r="93" ht="20" customHeight="1">
-      <c r="F93" s="34" t="n">
+      <c r="F93" t="n">
         <v>6533.269</v>
       </c>
-      <c r="G93" s="34" t="n">
+      <c r="G93" t="n">
         <v>7142.209</v>
       </c>
-      <c r="I93" s="34" t="n">
+      <c r="I93" t="n">
         <v>65</v>
       </c>
-      <c r="J93" s="34" t="n">
+      <c r="J93" t="n">
         <v>65</v>
       </c>
-      <c r="L93" s="34" t="n">
+      <c r="L93" t="n">
         <v>24</v>
       </c>
-      <c r="M93" s="34" t="n">
+      <c r="M93" t="n">
         <v>24</v>
       </c>
-      <c r="O93" s="34" t="n">
+      <c r="O93" t="n">
         <v>896</v>
       </c>
-      <c r="P93" s="34" t="n">
+      <c r="P93" t="n">
         <v>896</v>
       </c>
-      <c r="R93" s="76" t="n">
+      <c r="R93" t="n">
         <v>1</v>
       </c>
-      <c r="S93" s="76" t="n">
+      <c r="S93" t="n">
         <v>0.85</v>
       </c>
-      <c r="U93" s="34" t="n">
+      <c r="U93" t="n">
         <v>3.625</v>
       </c>
-      <c r="V93" s="34" t="n">
+      <c r="V93" t="n">
         <v>4</v>
       </c>
-      <c r="X93" s="34" t="n">
+      <c r="X93" t="n">
         <v>1.83</v>
       </c>
-      <c r="Y93" s="34" t="n">
+      <c r="Y93" t="n">
         <v>2.7</v>
       </c>
     </row>
     <row r="94" ht="20" customHeight="1">
-      <c r="F94" s="34" t="n">
+      <c r="F94" t="n">
         <v>6908.585</v>
       </c>
-      <c r="G94" s="34" t="n">
+      <c r="G94" t="n">
         <v>7350.49</v>
       </c>
-      <c r="I94" s="34" t="n">
+      <c r="I94" t="n">
         <v>65</v>
       </c>
-      <c r="J94" s="34" t="n">
+      <c r="J94" t="n">
         <v>65</v>
       </c>
-      <c r="L94" s="34" t="n">
+      <c r="L94" t="n">
         <v>25</v>
       </c>
-      <c r="M94" s="34" t="n">
+      <c r="M94" t="n">
         <v>25</v>
       </c>
-      <c r="O94" s="34" t="n">
+      <c r="O94" t="n">
         <v>896</v>
       </c>
-      <c r="P94" s="34" t="n">
+      <c r="P94" t="n">
         <v>896</v>
       </c>
-      <c r="R94" s="76" t="n">
+      <c r="R94" t="n">
         <v>1</v>
       </c>
-      <c r="S94" s="76" t="n">
+      <c r="S94" t="n">
         <v>0.85</v>
       </c>
-      <c r="U94" s="34" t="n">
+      <c r="U94" t="n">
         <v>3.625</v>
       </c>
-      <c r="V94" s="34" t="n">
+      <c r="V94" t="n">
         <v>4</v>
       </c>
-      <c r="X94" s="34" t="n">
+      <c r="X94" t="n">
         <v>1.949</v>
       </c>
-      <c r="Y94" s="34" t="n">
+      <c r="Y94" t="n">
         <v>2.871</v>
       </c>
     </row>
     <row r="95" ht="20" customHeight="1">
-      <c r="F95" s="34" t="n">
+      <c r="F95" t="n">
         <v>7293.975</v>
       </c>
-      <c r="G95" s="34" t="n">
+      <c r="G95" t="n">
         <v>7558.722</v>
       </c>
-      <c r="I95" s="34" t="n">
+      <c r="I95" t="n">
         <v>65</v>
       </c>
-      <c r="J95" s="34" t="n">
+      <c r="J95" t="n">
         <v>65</v>
       </c>
-      <c r="L95" s="34" t="n">
+      <c r="L95" t="n">
         <v>26</v>
       </c>
-      <c r="M95" s="34" t="n">
+      <c r="M95" t="n">
         <v>26</v>
       </c>
-      <c r="O95" s="34" t="n">
+      <c r="O95" t="n">
         <v>896</v>
       </c>
-      <c r="P95" s="34" t="n">
+      <c r="P95" t="n">
         <v>896</v>
       </c>
-      <c r="R95" s="76" t="n">
+      <c r="R95" t="n">
         <v>1</v>
       </c>
-      <c r="S95" s="76" t="n">
+      <c r="S95" t="n">
         <v>0.85</v>
       </c>
-      <c r="U95" s="34" t="n">
+      <c r="U95" t="n">
         <v>3.625</v>
       </c>
-      <c r="V95" s="34" t="n">
+      <c r="V95" t="n">
         <v>4</v>
       </c>
-      <c r="X95" s="34" t="n">
+      <c r="X95" t="n">
         <v>2.067</v>
       </c>
-      <c r="Y95" s="34" t="n">
+      <c r="Y95" t="n">
         <v>3.043</v>
       </c>
     </row>
     <row r="96" ht="20" customHeight="1">
-      <c r="F96" s="34" t="n">
+      <c r="F96" t="n">
         <v>7689.417</v>
       </c>
-      <c r="G96" s="34" t="n">
+      <c r="G96" t="n">
         <v>7766.905</v>
       </c>
-      <c r="I96" s="34" t="n">
+      <c r="I96" t="n">
         <v>65</v>
       </c>
-      <c r="J96" s="34" t="n">
+      <c r="J96" t="n">
         <v>65</v>
       </c>
-      <c r="L96" s="34" t="n">
+      <c r="L96" t="n">
         <v>27</v>
       </c>
-      <c r="M96" s="34" t="n">
+      <c r="M96" t="n">
         <v>27</v>
       </c>
-      <c r="O96" s="34" t="n">
+      <c r="O96" t="n">
         <v>896</v>
       </c>
-      <c r="P96" s="34" t="n">
+      <c r="P96" t="n">
         <v>896</v>
       </c>
-      <c r="R96" s="76" t="n">
+      <c r="R96" t="n">
         <v>1</v>
       </c>
-      <c r="S96" s="76" t="n">
+      <c r="S96" t="n">
         <v>0.85</v>
       </c>
-      <c r="U96" s="34" t="n">
+      <c r="U96" t="n">
         <v>3.625</v>
       </c>
-      <c r="V96" s="34" t="n">
+      <c r="V96" t="n">
         <v>4</v>
       </c>
-      <c r="X96" s="34" t="n">
+      <c r="X96" t="n">
         <v>2.186</v>
       </c>
-      <c r="Y96" s="34" t="n">
+      <c r="Y96" t="n">
         <v>3.214</v>
       </c>
     </row>
     <row r="97" ht="17.25" customHeight="1">
-      <c r="F97" s="34" t="n">
+      <c r="F97" t="n">
         <v>8094.892</v>
       </c>
-      <c r="G97" s="34" t="n">
+      <c r="G97" t="n">
         <v>7975.041</v>
       </c>
-      <c r="I97" s="34" t="n">
+      <c r="I97" t="n">
         <v>65</v>
       </c>
-      <c r="J97" s="34" t="n">
+      <c r="J97" t="n">
         <v>65</v>
       </c>
-      <c r="L97" s="34" t="n">
+      <c r="L97" t="n">
         <v>28</v>
       </c>
-      <c r="M97" s="34" t="n">
+      <c r="M97" t="n">
         <v>28</v>
       </c>
-      <c r="O97" s="34" t="n">
+      <c r="O97" t="n">
         <v>896</v>
       </c>
-      <c r="P97" s="34" t="n">
+      <c r="P97" t="n">
         <v>896</v>
       </c>
-      <c r="R97" s="76" t="n">
+      <c r="R97" t="n">
         <v>1</v>
       </c>
-      <c r="S97" s="76" t="n">
+      <c r="S97" t="n">
         <v>0.85</v>
       </c>
-      <c r="U97" s="34" t="n">
+      <c r="U97" t="n">
         <v>3.625</v>
       </c>
-      <c r="V97" s="34" t="n">
+      <c r="V97" t="n">
         <v>4</v>
       </c>
-      <c r="X97" s="34" t="n">
+      <c r="X97" t="n">
         <v>2.304</v>
       </c>
-      <c r="Y97" s="34" t="n">
+      <c r="Y97" t="n">
         <v>3.386</v>
       </c>
     </row>
     <row r="98" ht="17.25" customHeight="1">
-      <c r="F98" s="34" t="n">
+      <c r="F98" t="n">
         <v>8510.379999999999</v>
       </c>
-      <c r="G98" s="34" t="n">
+      <c r="G98" t="n">
         <v>8183.131</v>
       </c>
-      <c r="I98" s="34" t="n">
+      <c r="I98" t="n">
         <v>65</v>
       </c>
-      <c r="J98" s="34" t="n">
+      <c r="J98" t="n">
         <v>65</v>
       </c>
-      <c r="L98" s="34" t="n">
+      <c r="L98" t="n">
         <v>29</v>
       </c>
-      <c r="M98" s="34" t="n">
+      <c r="M98" t="n">
         <v>29</v>
       </c>
-      <c r="O98" s="34" t="n">
+      <c r="O98" t="n">
         <v>896</v>
       </c>
-      <c r="P98" s="34" t="n">
+      <c r="P98" t="n">
         <v>896</v>
       </c>
-      <c r="R98" s="76" t="n">
+      <c r="R98" t="n">
         <v>1</v>
       </c>
-      <c r="S98" s="76" t="n">
+      <c r="S98" t="n">
         <v>0.85</v>
       </c>
-      <c r="U98" s="34" t="n">
+      <c r="U98" t="n">
         <v>3.625</v>
       </c>
-      <c r="V98" s="34" t="n">
+      <c r="V98" t="n">
         <v>4</v>
       </c>
-      <c r="X98" s="34" t="n">
+      <c r="X98" t="n">
         <v>2.423</v>
       </c>
-      <c r="Y98" s="34" t="n">
+      <c r="Y98" t="n">
         <v>3.557</v>
       </c>
     </row>
     <row r="99" ht="17.25" customHeight="1">
-      <c r="F99" s="34" t="n">
+      <c r="F99" t="n">
         <v>8935.861999999999</v>
       </c>
-      <c r="G99" s="34" t="n">
+      <c r="G99" t="n">
         <v>8391.177</v>
       </c>
-      <c r="I99" s="34" t="n">
+      <c r="I99" t="n">
         <v>65</v>
       </c>
-      <c r="J99" s="34" t="n">
+      <c r="J99" t="n">
         <v>65</v>
       </c>
-      <c r="L99" s="34" t="n">
+      <c r="L99" t="n">
         <v>30</v>
       </c>
-      <c r="M99" s="34" t="n">
+      <c r="M99" t="n">
         <v>30</v>
       </c>
-      <c r="O99" s="34" t="n">
+      <c r="O99" t="n">
         <v>896</v>
       </c>
-      <c r="P99" s="34" t="n">
+      <c r="P99" t="n">
         <v>896</v>
       </c>
-      <c r="R99" s="76" t="n">
+      <c r="R99" t="n">
         <v>1</v>
       </c>
-      <c r="S99" s="76" t="n">
+      <c r="S99" t="n">
         <v>0.85</v>
       </c>
-      <c r="U99" s="34" t="n">
+      <c r="U99" t="n">
         <v>3.625</v>
       </c>
-      <c r="V99" s="34" t="n">
+      <c r="V99" t="n">
         <v>4</v>
       </c>
-      <c r="X99" s="34" t="n">
+      <c r="X99" t="n">
         <v>2.541</v>
       </c>
-      <c r="Y99" s="34" t="n">
+      <c r="Y99" t="n">
         <v>3.729</v>
       </c>
     </row>
     <row r="100" ht="17.25" customHeight="1">
-      <c r="F100" s="34" t="n">
+      <c r="F100" t="n">
         <v>9371.32</v>
       </c>
-      <c r="G100" s="34" t="n">
+      <c r="G100" t="n">
         <v>8599.179</v>
       </c>
-      <c r="I100" s="34" t="n">
+      <c r="I100" t="n">
         <v>65</v>
       </c>
-      <c r="J100" s="34" t="n">
+      <c r="J100" t="n">
         <v>65</v>
       </c>
-      <c r="L100" s="34" t="n">
+      <c r="L100" t="n">
         <v>31</v>
       </c>
-      <c r="M100" s="34" t="n">
+      <c r="M100" t="n">
         <v>31</v>
       </c>
-      <c r="O100" s="34" t="n">
+      <c r="O100" t="n">
         <v>896</v>
       </c>
-      <c r="P100" s="34" t="n">
+      <c r="P100" t="n">
         <v>896</v>
       </c>
-      <c r="R100" s="76" t="n">
+      <c r="R100" t="n">
         <v>1</v>
       </c>
-      <c r="S100" s="76" t="n">
+      <c r="S100" t="n">
         <v>0.85</v>
       </c>
-      <c r="U100" s="34" t="n">
+      <c r="U100" t="n">
         <v>3.625</v>
       </c>
-      <c r="V100" s="34" t="n">
+      <c r="V100" t="n">
         <v>4</v>
       </c>
-      <c r="X100" s="34" t="n">
+      <c r="X100" t="n">
         <v>2.66</v>
       </c>
-      <c r="Y100" s="34" t="n">
+      <c r="Y100" t="n">
         <v>3.9</v>
       </c>
     </row>
@@ -4310,9 +4240,7 @@
           <t>$</t>
         </is>
       </c>
-      <c r="H145" s="48" t="n">
-        <v>72.33336363636363</v>
-      </c>
+      <c r="H145" s="48" t="inlineStr"/>
       <c r="I145" s="60" t="inlineStr">
         <is>
           <t>$</t>

</xml_diff>